<commit_message>
Add robot settings to Create User
</commit_message>
<xml_diff>
--- a/Workbooks/JA/ユーザー.xlsx
+++ b/Workbooks/JA/ユーザー.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9537ACCD-FA1F-4643-973A-E8E31655ED02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABC55F9-43C9-4F4B-8946-A46B5D82C96D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58335" yWindow="735" windowWidth="36765" windowHeight="13335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="4940" windowWidth="30570" windowHeight="11930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>名</t>
   </si>
@@ -127,6 +127,65 @@
   </si>
   <si>
     <t>ユーザー名 *</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ログレベル</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>開発ログを許可</t>
+    <rPh sb="0" eb="2">
+      <t>かいはつ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>きょか</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>コンソールへログイン</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解像度の幅</t>
+    <rPh sb="0" eb="3">
+      <t>かいぞうど</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>はば</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解像度の高さ</t>
+    <rPh sb="0" eb="3">
+      <t>かいぞうど</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>たか</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解像度の階調</t>
+    <rPh sb="0" eb="3">
+      <t>かいぞうど</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>かいちょう</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>フォントスムージング</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>プロセスを自動ダウンロード</t>
+    <rPh sb="5" eb="7">
+      <t>じどう</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,83 +519,30 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="67">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1047,6 +1053,83 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="5"/>
@@ -1497,97 +1580,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="58" dataDxfId="56" totalsRowDxfId="54" headerRowBorderDxfId="57" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="66" dataDxfId="64" totalsRowDxfId="62" headerRowBorderDxfId="65" tableBorderDxfId="63">
   <autoFilter ref="A1:I201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{C22893F0-4B4D-460C-A013-95020C7502B4}" name="タイプ" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{1372863E-1574-486C-96A5-9F8A48DBEB17}" name="ID" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="ユーザー名" dataDxfId="50"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="名" totalsRowLabel="Total" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="姓" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="メールアドレス" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="組織単位名" totalsRowFunction="count" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="ロール名" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{73F4371D-09E6-432B-A8D2-FDF51584A3F9}" name="ステータス" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{C22893F0-4B4D-460C-A013-95020C7502B4}" name="タイプ" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{1372863E-1574-486C-96A5-9F8A48DBEB17}" name="ID" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="ユーザー名" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="名" totalsRowLabel="Total" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="姓" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="メールアドレス" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="組織単位名" totalsRowFunction="count" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="ロール名" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{73F4371D-09E6-432B-A8D2-FDF51584A3F9}" name="ステータス" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P201" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:P201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="16">
-    <tableColumn id="10" xr3:uid="{65749B7E-1278-4BF9-BE0E-B0B1A7EBF445}" name="ユーザー名 *" dataDxfId="41"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="名" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="姓" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="メールアドレス" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="組織単位名" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="ロール" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{4E111FFE-AC48-4FF2-B3E5-DEDE4EC1D531}" name="パスワード" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{6DE9A60B-D2AA-4C5B-9D19-151C1E73E0AC}" name="ドメイン\ユーザ名 - Attended ロボット" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{262304B2-69B6-47FC-833F-5922ED105520}" name="ライセンスの種類 - Attended ロボット" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{42564DA4-8D53-4C1B-9C2C-4BE92DD00FFC}" name="個人のワークスペースを作成 - Attended ロボット" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{49DD615B-15C2-4B9A-960E-9A70F1B8C51E}" name="スタンドアロンライセンス - Attended ロボット" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{B5515926-7E95-4BDC-B434-092F68C9E676}" name="ドメイン\ユーザー名 - Unattended ロボット" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{1EFF2166-C43F-4EFE-A90C-FFD898ED903B}" name="パスワード - Unattended Robot" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{E40F7CE9-454E-4944-9C0F-78161314E5AC}" name="同時接続実行を無効化 - Unattended Robot" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="ID" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{08B4DCAC-6628-4928-B533-CE43508622D2}" name="結果" dataDxfId="33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:X201" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+  <autoFilter ref="A1:X201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="24">
+    <tableColumn id="10" xr3:uid="{65749B7E-1278-4BF9-BE0E-B0B1A7EBF445}" name="ユーザー名 *" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="名" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="姓" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="メールアドレス" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="組織単位名" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="ロール" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{4E111FFE-AC48-4FF2-B3E5-DEDE4EC1D531}" name="パスワード" dataDxfId="43"/>
+    <tableColumn id="14" xr3:uid="{6DE9A60B-D2AA-4C5B-9D19-151C1E73E0AC}" name="ドメイン\ユーザ名 - Attended ロボット" dataDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{262304B2-69B6-47FC-833F-5922ED105520}" name="ライセンスの種類 - Attended ロボット" dataDxfId="41"/>
+    <tableColumn id="15" xr3:uid="{42564DA4-8D53-4C1B-9C2C-4BE92DD00FFC}" name="個人のワークスペースを作成 - Attended ロボット" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{49DD615B-15C2-4B9A-960E-9A70F1B8C51E}" name="スタンドアロンライセンス - Attended ロボット" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{B5515926-7E95-4BDC-B434-092F68C9E676}" name="ドメイン\ユーザー名 - Unattended ロボット" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{1EFF2166-C43F-4EFE-A90C-FFD898ED903B}" name="パスワード - Unattended Robot" dataDxfId="37"/>
+    <tableColumn id="17" xr3:uid="{E40F7CE9-454E-4944-9C0F-78161314E5AC}" name="同時接続実行を無効化 - Unattended Robot" dataDxfId="36"/>
+    <tableColumn id="24" xr3:uid="{4737097B-807F-467E-994B-823169C8851E}" name="ログレベル" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{F4F5E00E-44D5-478B-9E16-1E0836A97A31}" name="開発ログを許可" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{54CE7D6A-8149-4FF1-856C-0297F6C4EA6A}" name="コンソールへログイン" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{981701E3-426C-4D88-A3C1-45F9E3D28795}" name="解像度の幅" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{9DC42AD1-736C-4BEB-A7A8-35E20A7368C1}" name="解像度の高さ" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{45F1E31B-C2C4-4911-8745-575C838381F3}" name="解像度の階調" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{433CEED5-AD86-4341-87B3-24E355BD37E2}" name="フォントスムージング" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{ABE2AD9D-F7D1-4BD9-B771-C5E569C50B19}" name="プロセスを自動ダウンロード" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="ID" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{08B4DCAC-6628-4928-B533-CE43508622D2}" name="結果" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:G201" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:G201" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:G201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{01450210-36BE-4B28-9B3B-758A2770B142}" name="ID" dataDxfId="30"/>
-    <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="名" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="姓" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="メールアドレス" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{310BA8C6-70B4-40F4-B90F-2C40BB19BC10}" name="ステータス" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="パスワード" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{E7804193-086E-4884-9B07-86C7E77E0835}" name="結果" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{01450210-36BE-4B28-9B3B-758A2770B142}" name="ID" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="名" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="姓" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="メールアドレス" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{310BA8C6-70B4-40F4-B90F-2C40BB19BC10}" name="ステータス" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="パスワード" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{E7804193-086E-4884-9B07-86C7E77E0835}" name="結果" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C201" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C201" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:C201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID" dataDxfId="21"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ユーザー名" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="結果" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ユーザー名" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="結果" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9A9C6F0D-2E14-43CF-BA3F-71838E8A8593}" name="Table1367" displayName="Table1367" ref="A1:D201" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9A9C6F0D-2E14-43CF-BA3F-71838E8A8593}" name="Table1367" displayName="Table1367" ref="A1:D201" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EB9188D5-49DF-4F54-A843-A55D3E2C1BE7}" name="ユーザー ID" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{85E99034-1CC5-49C9-990E-916A8CEEC70B}" name="追加されるロール名" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{CE37118B-AB12-42D8-BD3F-A9948E262C56}" name="削除されるロール名" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{C8060084-F897-4904-AA9C-11EEA24740A4}" name="結果" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{EB9188D5-49DF-4F54-A843-A55D3E2C1BE7}" name="ユーザー ID" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{85E99034-1CC5-49C9-990E-916A8CEEC70B}" name="追加されるロール名" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{CE37118B-AB12-42D8-BD3F-A9948E262C56}" name="削除されるロール名" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{C8060084-F897-4904-AA9C-11EEA24740A4}" name="結果" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F4943553-1107-4ABF-92F1-3D44259ECE3F}" name="Table136" displayName="Table136" ref="A1:D201" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F4943553-1107-4ABF-92F1-3D44259ECE3F}" name="Table136" displayName="Table136" ref="A1:D201" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AECF12CD-DED5-4EAC-990D-027FA15BD77B}" name="ユーザーID" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{386847AF-7B54-40AC-B632-9092A64C412D}" name="追加される組織単位名" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{927EBCB0-231E-4AA5-99D9-8C13EE557A37}" name="削除される組織単位名" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{85CBEB5B-343A-4F2F-8DE9-C961C7CE168C}" name="結果" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{AECF12CD-DED5-4EAC-990D-027FA15BD77B}" name="ユーザーID" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{386847AF-7B54-40AC-B632-9092A64C412D}" name="追加される組織単位名" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{927EBCB0-231E-4AA5-99D9-8C13EE557A37}" name="削除される組織単位名" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{85CBEB5B-343A-4F2F-8DE9-C961C7CE168C}" name="結果" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4121,10 +4212,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P201"/>
+  <dimension ref="A1:X201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -4134,13 +4225,13 @@
     <col min="5" max="6" width="45.6640625" style="29" customWidth="1"/>
     <col min="7" max="7" width="25.5" style="29" customWidth="1"/>
     <col min="8" max="14" width="25.5" style="2" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" style="31" customWidth="1"/>
-    <col min="16" max="16" width="45.6640625" style="31" customWidth="1"/>
-    <col min="17" max="17" width="11.25" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="8.75" style="2"/>
+    <col min="15" max="22" width="25.75" style="2" customWidth="1"/>
+    <col min="23" max="23" width="11.25" style="31" customWidth="1"/>
+    <col min="24" max="24" width="8.75" style="31"/>
+    <col min="25" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:24" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -4183,14 +4274,38 @@
       <c r="N1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="X1" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4198,10 +4313,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="12"/>
       <c r="G2" s="25"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -4209,10 +4324,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="12"/>
       <c r="G3" s="25"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -4220,10 +4335,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
       <c r="G4" s="25"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -4231,10 +4346,10 @@
       <c r="E5" s="8"/>
       <c r="F5" s="12"/>
       <c r="G5" s="25"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -4242,10 +4357,10 @@
       <c r="E6" s="8"/>
       <c r="F6" s="12"/>
       <c r="G6" s="25"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -4253,10 +4368,10 @@
       <c r="E7" s="8"/>
       <c r="F7" s="12"/>
       <c r="G7" s="25"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -4264,10 +4379,10 @@
       <c r="E8" s="8"/>
       <c r="F8" s="12"/>
       <c r="G8" s="25"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -4275,10 +4390,10 @@
       <c r="E9" s="8"/>
       <c r="F9" s="12"/>
       <c r="G9" s="25"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -4286,10 +4401,10 @@
       <c r="E10" s="8"/>
       <c r="F10" s="12"/>
       <c r="G10" s="25"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -4297,10 +4412,10 @@
       <c r="E11" s="8"/>
       <c r="F11" s="12"/>
       <c r="G11" s="25"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -4308,10 +4423,10 @@
       <c r="E12" s="8"/>
       <c r="F12" s="12"/>
       <c r="G12" s="25"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -4319,10 +4434,10 @@
       <c r="E13" s="8"/>
       <c r="F13" s="12"/>
       <c r="G13" s="25"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -4330,10 +4445,10 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -4341,10 +4456,10 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -4352,10 +4467,10 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -4363,10 +4478,10 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -4374,10 +4489,10 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -4385,10 +4500,10 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -4396,10 +4511,10 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -4407,10 +4522,10 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="9"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -4418,10 +4533,10 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="9"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -4429,10 +4544,10 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -4440,10 +4555,10 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -4451,10 +4566,10 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -4462,10 +4577,10 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -4473,10 +4588,10 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -4484,10 +4599,10 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="9"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -4495,10 +4610,10 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -4506,10 +4621,10 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -4517,10 +4632,10 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -4528,10 +4643,10 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="9"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -4539,10 +4654,10 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -4550,10 +4665,10 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -4561,10 +4676,10 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -4572,10 +4687,10 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -4583,10 +4698,10 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -4594,10 +4709,10 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -4605,10 +4720,10 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -4616,10 +4731,10 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -4627,10 +4742,10 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -4638,10 +4753,10 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -4649,10 +4764,10 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -4660,10 +4775,10 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -4671,10 +4786,10 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="9"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -4682,10 +4797,10 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="9"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -4693,10 +4808,10 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W47" s="3"/>
+      <c r="X47" s="3"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -4704,10 +4819,10 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="9"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -4715,10 +4830,10 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="9"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -4726,10 +4841,10 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="9"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -4737,10 +4852,10 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -4748,10 +4863,10 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="9"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -4759,10 +4874,10 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="9"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W53" s="3"/>
+      <c r="X53" s="3"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -4770,10 +4885,10 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="9"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W54" s="3"/>
+      <c r="X54" s="3"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -4781,10 +4896,10 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W55" s="3"/>
+      <c r="X55" s="3"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -4792,10 +4907,10 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -4803,10 +4918,10 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="9"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W57" s="3"/>
+      <c r="X57" s="3"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -4814,10 +4929,10 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W58" s="3"/>
+      <c r="X58" s="3"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -4825,10 +4940,10 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="9"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W59" s="3"/>
+      <c r="X59" s="3"/>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -4836,10 +4951,10 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="9"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W60" s="3"/>
+      <c r="X60" s="3"/>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -4847,10 +4962,10 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="9"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W61" s="3"/>
+      <c r="X61" s="3"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -4858,10 +4973,10 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="9"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="3"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W62" s="3"/>
+      <c r="X62" s="3"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -4869,10 +4984,10 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="9"/>
-      <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -4880,10 +4995,10 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="9"/>
-      <c r="O64" s="3"/>
-      <c r="P64" s="3"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W64" s="3"/>
+      <c r="X64" s="3"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -4891,10 +5006,10 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="9"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W65" s="3"/>
+      <c r="X65" s="3"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -4902,10 +5017,10 @@
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="9"/>
-      <c r="O66" s="3"/>
-      <c r="P66" s="3"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W66" s="3"/>
+      <c r="X66" s="3"/>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -4913,10 +5028,10 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="9"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W67" s="3"/>
+      <c r="X67" s="3"/>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -4924,10 +5039,10 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="9"/>
-      <c r="O68" s="3"/>
-      <c r="P68" s="3"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -4935,10 +5050,10 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="9"/>
-      <c r="O69" s="3"/>
-      <c r="P69" s="3"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W69" s="3"/>
+      <c r="X69" s="3"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -4946,10 +5061,10 @@
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="9"/>
-      <c r="O70" s="3"/>
-      <c r="P70" s="3"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W70" s="3"/>
+      <c r="X70" s="3"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -4957,10 +5072,10 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="9"/>
-      <c r="O71" s="3"/>
-      <c r="P71" s="3"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W71" s="3"/>
+      <c r="X71" s="3"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -4968,10 +5083,10 @@
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="9"/>
-      <c r="O72" s="3"/>
-      <c r="P72" s="3"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W72" s="3"/>
+      <c r="X72" s="3"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -4979,10 +5094,10 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="9"/>
-      <c r="O73" s="3"/>
-      <c r="P73" s="3"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W73" s="3"/>
+      <c r="X73" s="3"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -4990,10 +5105,10 @@
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="9"/>
-      <c r="O74" s="3"/>
-      <c r="P74" s="3"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W74" s="3"/>
+      <c r="X74" s="3"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -5001,10 +5116,10 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="9"/>
-      <c r="O75" s="3"/>
-      <c r="P75" s="3"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W75" s="3"/>
+      <c r="X75" s="3"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -5012,10 +5127,10 @@
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="9"/>
-      <c r="O76" s="3"/>
-      <c r="P76" s="3"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W76" s="3"/>
+      <c r="X76" s="3"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -5023,10 +5138,10 @@
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
       <c r="G77" s="9"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W77" s="3"/>
+      <c r="X77" s="3"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -5034,10 +5149,10 @@
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
       <c r="G78" s="9"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="3"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W78" s="3"/>
+      <c r="X78" s="3"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -5045,10 +5160,10 @@
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="9"/>
-      <c r="O79" s="3"/>
-      <c r="P79" s="3"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W79" s="3"/>
+      <c r="X79" s="3"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
@@ -5056,10 +5171,10 @@
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
       <c r="G80" s="9"/>
-      <c r="O80" s="3"/>
-      <c r="P80" s="3"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W80" s="3"/>
+      <c r="X80" s="3"/>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -5067,10 +5182,10 @@
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
       <c r="G81" s="9"/>
-      <c r="O81" s="3"/>
-      <c r="P81" s="3"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W81" s="3"/>
+      <c r="X81" s="3"/>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -5078,10 +5193,10 @@
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
       <c r="G82" s="9"/>
-      <c r="O82" s="3"/>
-      <c r="P82" s="3"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W82" s="3"/>
+      <c r="X82" s="3"/>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -5089,10 +5204,10 @@
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
       <c r="G83" s="9"/>
-      <c r="O83" s="3"/>
-      <c r="P83" s="3"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W83" s="3"/>
+      <c r="X83" s="3"/>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -5100,10 +5215,10 @@
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
       <c r="G84" s="9"/>
-      <c r="O84" s="3"/>
-      <c r="P84" s="3"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W84" s="3"/>
+      <c r="X84" s="3"/>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
@@ -5111,10 +5226,10 @@
       <c r="E85" s="8"/>
       <c r="F85" s="8"/>
       <c r="G85" s="9"/>
-      <c r="O85" s="3"/>
-      <c r="P85" s="3"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W85" s="3"/>
+      <c r="X85" s="3"/>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -5122,10 +5237,10 @@
       <c r="E86" s="8"/>
       <c r="F86" s="8"/>
       <c r="G86" s="9"/>
-      <c r="O86" s="3"/>
-      <c r="P86" s="3"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W86" s="3"/>
+      <c r="X86" s="3"/>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
@@ -5133,10 +5248,10 @@
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
       <c r="G87" s="9"/>
-      <c r="O87" s="3"/>
-      <c r="P87" s="3"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W87" s="3"/>
+      <c r="X87" s="3"/>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
@@ -5144,10 +5259,10 @@
       <c r="E88" s="8"/>
       <c r="F88" s="8"/>
       <c r="G88" s="9"/>
-      <c r="O88" s="3"/>
-      <c r="P88" s="3"/>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W88" s="3"/>
+      <c r="X88" s="3"/>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
@@ -5155,10 +5270,10 @@
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
       <c r="G89" s="9"/>
-      <c r="O89" s="3"/>
-      <c r="P89" s="3"/>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W89" s="3"/>
+      <c r="X89" s="3"/>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
@@ -5166,10 +5281,10 @@
       <c r="E90" s="8"/>
       <c r="F90" s="8"/>
       <c r="G90" s="9"/>
-      <c r="O90" s="3"/>
-      <c r="P90" s="3"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W90" s="3"/>
+      <c r="X90" s="3"/>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
@@ -5177,10 +5292,10 @@
       <c r="E91" s="8"/>
       <c r="F91" s="8"/>
       <c r="G91" s="9"/>
-      <c r="O91" s="3"/>
-      <c r="P91" s="3"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W91" s="3"/>
+      <c r="X91" s="3"/>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
@@ -5188,10 +5303,10 @@
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
       <c r="G92" s="9"/>
-      <c r="O92" s="3"/>
-      <c r="P92" s="3"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W92" s="3"/>
+      <c r="X92" s="3"/>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -5199,10 +5314,10 @@
       <c r="E93" s="8"/>
       <c r="F93" s="8"/>
       <c r="G93" s="9"/>
-      <c r="O93" s="3"/>
-      <c r="P93" s="3"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W93" s="3"/>
+      <c r="X93" s="3"/>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -5210,10 +5325,10 @@
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
       <c r="G94" s="9"/>
-      <c r="O94" s="3"/>
-      <c r="P94" s="3"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W94" s="3"/>
+      <c r="X94" s="3"/>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
@@ -5221,10 +5336,10 @@
       <c r="E95" s="8"/>
       <c r="F95" s="8"/>
       <c r="G95" s="9"/>
-      <c r="O95" s="3"/>
-      <c r="P95" s="3"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W95" s="3"/>
+      <c r="X95" s="3"/>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
@@ -5232,10 +5347,10 @@
       <c r="E96" s="8"/>
       <c r="F96" s="8"/>
       <c r="G96" s="9"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W96" s="3"/>
+      <c r="X96" s="3"/>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
@@ -5243,10 +5358,10 @@
       <c r="E97" s="8"/>
       <c r="F97" s="8"/>
       <c r="G97" s="9"/>
-      <c r="O97" s="3"/>
-      <c r="P97" s="3"/>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W97" s="3"/>
+      <c r="X97" s="3"/>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
@@ -5254,10 +5369,10 @@
       <c r="E98" s="8"/>
       <c r="F98" s="8"/>
       <c r="G98" s="9"/>
-      <c r="O98" s="3"/>
-      <c r="P98" s="3"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W98" s="3"/>
+      <c r="X98" s="3"/>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
@@ -5265,10 +5380,10 @@
       <c r="E99" s="8"/>
       <c r="F99" s="8"/>
       <c r="G99" s="9"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W99" s="3"/>
+      <c r="X99" s="3"/>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -5276,10 +5391,10 @@
       <c r="E100" s="8"/>
       <c r="F100" s="8"/>
       <c r="G100" s="9"/>
-      <c r="O100" s="3"/>
-      <c r="P100" s="3"/>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W100" s="3"/>
+      <c r="X100" s="3"/>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="8"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
@@ -5287,10 +5402,10 @@
       <c r="E101" s="8"/>
       <c r="F101" s="8"/>
       <c r="G101" s="9"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W101" s="3"/>
+      <c r="X101" s="3"/>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -5298,10 +5413,10 @@
       <c r="E102" s="8"/>
       <c r="F102" s="8"/>
       <c r="G102" s="8"/>
-      <c r="O102" s="3"/>
-      <c r="P102" s="3"/>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W102" s="3"/>
+      <c r="X102" s="3"/>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -5309,10 +5424,10 @@
       <c r="E103" s="8"/>
       <c r="F103" s="8"/>
       <c r="G103" s="8"/>
-      <c r="O103" s="3"/>
-      <c r="P103" s="3"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W103" s="3"/>
+      <c r="X103" s="3"/>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
@@ -5320,10 +5435,10 @@
       <c r="E104" s="8"/>
       <c r="F104" s="8"/>
       <c r="G104" s="8"/>
-      <c r="O104" s="3"/>
-      <c r="P104" s="3"/>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W104" s="3"/>
+      <c r="X104" s="3"/>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
@@ -5331,10 +5446,10 @@
       <c r="E105" s="8"/>
       <c r="F105" s="8"/>
       <c r="G105" s="8"/>
-      <c r="O105" s="3"/>
-      <c r="P105" s="3"/>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W105" s="3"/>
+      <c r="X105" s="3"/>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="8"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -5342,10 +5457,10 @@
       <c r="E106" s="8"/>
       <c r="F106" s="8"/>
       <c r="G106" s="8"/>
-      <c r="O106" s="3"/>
-      <c r="P106" s="3"/>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W106" s="3"/>
+      <c r="X106" s="3"/>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="8"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
@@ -5353,10 +5468,10 @@
       <c r="E107" s="8"/>
       <c r="F107" s="8"/>
       <c r="G107" s="8"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3"/>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W107" s="3"/>
+      <c r="X107" s="3"/>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
@@ -5364,10 +5479,10 @@
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
       <c r="G108" s="8"/>
-      <c r="O108" s="3"/>
-      <c r="P108" s="3"/>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W108" s="3"/>
+      <c r="X108" s="3"/>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
@@ -5375,10 +5490,10 @@
       <c r="E109" s="8"/>
       <c r="F109" s="8"/>
       <c r="G109" s="8"/>
-      <c r="O109" s="3"/>
-      <c r="P109" s="3"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W109" s="3"/>
+      <c r="X109" s="3"/>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
@@ -5386,10 +5501,10 @@
       <c r="E110" s="8"/>
       <c r="F110" s="8"/>
       <c r="G110" s="8"/>
-      <c r="O110" s="3"/>
-      <c r="P110" s="3"/>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W110" s="3"/>
+      <c r="X110" s="3"/>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
@@ -5397,10 +5512,10 @@
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
       <c r="G111" s="8"/>
-      <c r="O111" s="3"/>
-      <c r="P111" s="3"/>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W111" s="3"/>
+      <c r="X111" s="3"/>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
@@ -5408,10 +5523,10 @@
       <c r="E112" s="8"/>
       <c r="F112" s="8"/>
       <c r="G112" s="8"/>
-      <c r="O112" s="3"/>
-      <c r="P112" s="3"/>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W112" s="3"/>
+      <c r="X112" s="3"/>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
@@ -5419,10 +5534,10 @@
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
       <c r="G113" s="8"/>
-      <c r="O113" s="3"/>
-      <c r="P113" s="3"/>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W113" s="3"/>
+      <c r="X113" s="3"/>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="8"/>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
@@ -5430,10 +5545,10 @@
       <c r="E114" s="8"/>
       <c r="F114" s="8"/>
       <c r="G114" s="8"/>
-      <c r="O114" s="3"/>
-      <c r="P114" s="3"/>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W114" s="3"/>
+      <c r="X114" s="3"/>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="8"/>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
@@ -5441,10 +5556,10 @@
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
       <c r="G115" s="8"/>
-      <c r="O115" s="3"/>
-      <c r="P115" s="3"/>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W115" s="3"/>
+      <c r="X115" s="3"/>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
@@ -5452,10 +5567,10 @@
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
       <c r="G116" s="8"/>
-      <c r="O116" s="3"/>
-      <c r="P116" s="3"/>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W116" s="3"/>
+      <c r="X116" s="3"/>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="8"/>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
@@ -5463,10 +5578,10 @@
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
       <c r="G117" s="8"/>
-      <c r="O117" s="3"/>
-      <c r="P117" s="3"/>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W117" s="3"/>
+      <c r="X117" s="3"/>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
@@ -5474,10 +5589,10 @@
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
       <c r="G118" s="8"/>
-      <c r="O118" s="3"/>
-      <c r="P118" s="3"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W118" s="3"/>
+      <c r="X118" s="3"/>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
@@ -5485,10 +5600,10 @@
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
       <c r="G119" s="8"/>
-      <c r="O119" s="3"/>
-      <c r="P119" s="3"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W119" s="3"/>
+      <c r="X119" s="3"/>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="8"/>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
@@ -5496,10 +5611,10 @@
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
       <c r="G120" s="8"/>
-      <c r="O120" s="3"/>
-      <c r="P120" s="3"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W120" s="3"/>
+      <c r="X120" s="3"/>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="8"/>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
@@ -5507,10 +5622,10 @@
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
       <c r="G121" s="8"/>
-      <c r="O121" s="3"/>
-      <c r="P121" s="3"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W121" s="3"/>
+      <c r="X121" s="3"/>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
@@ -5518,10 +5633,10 @@
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
       <c r="G122" s="8"/>
-      <c r="O122" s="3"/>
-      <c r="P122" s="3"/>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W122" s="3"/>
+      <c r="X122" s="3"/>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
@@ -5529,10 +5644,10 @@
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
       <c r="G123" s="8"/>
-      <c r="O123" s="3"/>
-      <c r="P123" s="3"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W123" s="3"/>
+      <c r="X123" s="3"/>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
@@ -5540,10 +5655,10 @@
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
       <c r="G124" s="8"/>
-      <c r="O124" s="3"/>
-      <c r="P124" s="3"/>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W124" s="3"/>
+      <c r="X124" s="3"/>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="8"/>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
@@ -5551,10 +5666,10 @@
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
       <c r="G125" s="8"/>
-      <c r="O125" s="3"/>
-      <c r="P125" s="3"/>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W125" s="3"/>
+      <c r="X125" s="3"/>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="8"/>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
@@ -5562,10 +5677,10 @@
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
       <c r="G126" s="8"/>
-      <c r="O126" s="3"/>
-      <c r="P126" s="3"/>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W126" s="3"/>
+      <c r="X126" s="3"/>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="8"/>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
@@ -5573,10 +5688,10 @@
       <c r="E127" s="8"/>
       <c r="F127" s="8"/>
       <c r="G127" s="8"/>
-      <c r="O127" s="3"/>
-      <c r="P127" s="3"/>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W127" s="3"/>
+      <c r="X127" s="3"/>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="8"/>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
@@ -5584,10 +5699,10 @@
       <c r="E128" s="8"/>
       <c r="F128" s="8"/>
       <c r="G128" s="8"/>
-      <c r="O128" s="3"/>
-      <c r="P128" s="3"/>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W128" s="3"/>
+      <c r="X128" s="3"/>
+    </row>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="8"/>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -5595,10 +5710,10 @@
       <c r="E129" s="8"/>
       <c r="F129" s="8"/>
       <c r="G129" s="8"/>
-      <c r="O129" s="3"/>
-      <c r="P129" s="3"/>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W129" s="3"/>
+      <c r="X129" s="3"/>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="8"/>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
@@ -5606,10 +5721,10 @@
       <c r="E130" s="8"/>
       <c r="F130" s="8"/>
       <c r="G130" s="8"/>
-      <c r="O130" s="3"/>
-      <c r="P130" s="3"/>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W130" s="3"/>
+      <c r="X130" s="3"/>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="8"/>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
@@ -5617,10 +5732,10 @@
       <c r="E131" s="8"/>
       <c r="F131" s="8"/>
       <c r="G131" s="8"/>
-      <c r="O131" s="3"/>
-      <c r="P131" s="3"/>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W131" s="3"/>
+      <c r="X131" s="3"/>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="8"/>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
@@ -5628,10 +5743,10 @@
       <c r="E132" s="8"/>
       <c r="F132" s="8"/>
       <c r="G132" s="8"/>
-      <c r="O132" s="3"/>
-      <c r="P132" s="3"/>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W132" s="3"/>
+      <c r="X132" s="3"/>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="8"/>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
@@ -5639,10 +5754,10 @@
       <c r="E133" s="8"/>
       <c r="F133" s="8"/>
       <c r="G133" s="8"/>
-      <c r="O133" s="3"/>
-      <c r="P133" s="3"/>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W133" s="3"/>
+      <c r="X133" s="3"/>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="8"/>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
@@ -5650,10 +5765,10 @@
       <c r="E134" s="8"/>
       <c r="F134" s="8"/>
       <c r="G134" s="8"/>
-      <c r="O134" s="3"/>
-      <c r="P134" s="3"/>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W134" s="3"/>
+      <c r="X134" s="3"/>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="8"/>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
@@ -5661,10 +5776,10 @@
       <c r="E135" s="8"/>
       <c r="F135" s="8"/>
       <c r="G135" s="8"/>
-      <c r="O135" s="3"/>
-      <c r="P135" s="3"/>
-    </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W135" s="3"/>
+      <c r="X135" s="3"/>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
@@ -5672,10 +5787,10 @@
       <c r="E136" s="8"/>
       <c r="F136" s="8"/>
       <c r="G136" s="8"/>
-      <c r="O136" s="3"/>
-      <c r="P136" s="3"/>
-    </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W136" s="3"/>
+      <c r="X136" s="3"/>
+    </row>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="8"/>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
@@ -5683,10 +5798,10 @@
       <c r="E137" s="8"/>
       <c r="F137" s="8"/>
       <c r="G137" s="8"/>
-      <c r="O137" s="3"/>
-      <c r="P137" s="3"/>
-    </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W137" s="3"/>
+      <c r="X137" s="3"/>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
@@ -5694,10 +5809,10 @@
       <c r="E138" s="8"/>
       <c r="F138" s="8"/>
       <c r="G138" s="8"/>
-      <c r="O138" s="3"/>
-      <c r="P138" s="3"/>
-    </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W138" s="3"/>
+      <c r="X138" s="3"/>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="8"/>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
@@ -5705,10 +5820,10 @@
       <c r="E139" s="8"/>
       <c r="F139" s="8"/>
       <c r="G139" s="8"/>
-      <c r="O139" s="3"/>
-      <c r="P139" s="3"/>
-    </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W139" s="3"/>
+      <c r="X139" s="3"/>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="8"/>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
@@ -5716,10 +5831,10 @@
       <c r="E140" s="8"/>
       <c r="F140" s="8"/>
       <c r="G140" s="8"/>
-      <c r="O140" s="3"/>
-      <c r="P140" s="3"/>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W140" s="3"/>
+      <c r="X140" s="3"/>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="8"/>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
@@ -5727,10 +5842,10 @@
       <c r="E141" s="8"/>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
-      <c r="O141" s="3"/>
-      <c r="P141" s="3"/>
-    </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W141" s="3"/>
+      <c r="X141" s="3"/>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
@@ -5738,10 +5853,10 @@
       <c r="E142" s="8"/>
       <c r="F142" s="8"/>
       <c r="G142" s="8"/>
-      <c r="O142" s="3"/>
-      <c r="P142" s="3"/>
-    </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W142" s="3"/>
+      <c r="X142" s="3"/>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -5749,10 +5864,10 @@
       <c r="E143" s="8"/>
       <c r="F143" s="8"/>
       <c r="G143" s="8"/>
-      <c r="O143" s="3"/>
-      <c r="P143" s="3"/>
-    </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W143" s="3"/>
+      <c r="X143" s="3"/>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
@@ -5760,10 +5875,10 @@
       <c r="E144" s="8"/>
       <c r="F144" s="8"/>
       <c r="G144" s="8"/>
-      <c r="O144" s="3"/>
-      <c r="P144" s="3"/>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W144" s="3"/>
+      <c r="X144" s="3"/>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="8"/>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
@@ -5771,10 +5886,10 @@
       <c r="E145" s="8"/>
       <c r="F145" s="8"/>
       <c r="G145" s="8"/>
-      <c r="O145" s="3"/>
-      <c r="P145" s="3"/>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W145" s="3"/>
+      <c r="X145" s="3"/>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
@@ -5782,10 +5897,10 @@
       <c r="E146" s="8"/>
       <c r="F146" s="8"/>
       <c r="G146" s="8"/>
-      <c r="O146" s="3"/>
-      <c r="P146" s="3"/>
-    </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W146" s="3"/>
+      <c r="X146" s="3"/>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="8"/>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
@@ -5793,10 +5908,10 @@
       <c r="E147" s="8"/>
       <c r="F147" s="8"/>
       <c r="G147" s="8"/>
-      <c r="O147" s="3"/>
-      <c r="P147" s="3"/>
-    </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W147" s="3"/>
+      <c r="X147" s="3"/>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
@@ -5804,10 +5919,10 @@
       <c r="E148" s="8"/>
       <c r="F148" s="8"/>
       <c r="G148" s="8"/>
-      <c r="O148" s="3"/>
-      <c r="P148" s="3"/>
-    </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W148" s="3"/>
+      <c r="X148" s="3"/>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
@@ -5815,10 +5930,10 @@
       <c r="E149" s="8"/>
       <c r="F149" s="8"/>
       <c r="G149" s="8"/>
-      <c r="O149" s="3"/>
-      <c r="P149" s="3"/>
-    </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W149" s="3"/>
+      <c r="X149" s="3"/>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="8"/>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
@@ -5826,10 +5941,10 @@
       <c r="E150" s="8"/>
       <c r="F150" s="8"/>
       <c r="G150" s="8"/>
-      <c r="O150" s="3"/>
-      <c r="P150" s="3"/>
-    </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W150" s="3"/>
+      <c r="X150" s="3"/>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="8"/>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
@@ -5837,10 +5952,10 @@
       <c r="E151" s="8"/>
       <c r="F151" s="8"/>
       <c r="G151" s="8"/>
-      <c r="O151" s="3"/>
-      <c r="P151" s="3"/>
-    </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W151" s="3"/>
+      <c r="X151" s="3"/>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="8"/>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
@@ -5848,10 +5963,10 @@
       <c r="E152" s="8"/>
       <c r="F152" s="8"/>
       <c r="G152" s="8"/>
-      <c r="O152" s="3"/>
-      <c r="P152" s="3"/>
-    </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W152" s="3"/>
+      <c r="X152" s="3"/>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="8"/>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
@@ -5859,10 +5974,10 @@
       <c r="E153" s="8"/>
       <c r="F153" s="8"/>
       <c r="G153" s="8"/>
-      <c r="O153" s="3"/>
-      <c r="P153" s="3"/>
-    </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W153" s="3"/>
+      <c r="X153" s="3"/>
+    </row>
+    <row r="154" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
@@ -5870,10 +5985,10 @@
       <c r="E154" s="8"/>
       <c r="F154" s="8"/>
       <c r="G154" s="8"/>
-      <c r="O154" s="3"/>
-      <c r="P154" s="3"/>
-    </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W154" s="3"/>
+      <c r="X154" s="3"/>
+    </row>
+    <row r="155" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="8"/>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
@@ -5881,10 +5996,10 @@
       <c r="E155" s="8"/>
       <c r="F155" s="8"/>
       <c r="G155" s="8"/>
-      <c r="O155" s="3"/>
-      <c r="P155" s="3"/>
-    </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W155" s="3"/>
+      <c r="X155" s="3"/>
+    </row>
+    <row r="156" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
@@ -5892,10 +6007,10 @@
       <c r="E156" s="8"/>
       <c r="F156" s="8"/>
       <c r="G156" s="8"/>
-      <c r="O156" s="3"/>
-      <c r="P156" s="3"/>
-    </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W156" s="3"/>
+      <c r="X156" s="3"/>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
@@ -5903,10 +6018,10 @@
       <c r="E157" s="8"/>
       <c r="F157" s="8"/>
       <c r="G157" s="8"/>
-      <c r="O157" s="3"/>
-      <c r="P157" s="3"/>
-    </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W157" s="3"/>
+      <c r="X157" s="3"/>
+    </row>
+    <row r="158" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="8"/>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
@@ -5914,10 +6029,10 @@
       <c r="E158" s="8"/>
       <c r="F158" s="8"/>
       <c r="G158" s="8"/>
-      <c r="O158" s="3"/>
-      <c r="P158" s="3"/>
-    </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W158" s="3"/>
+      <c r="X158" s="3"/>
+    </row>
+    <row r="159" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="8"/>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
@@ -5925,10 +6040,10 @@
       <c r="E159" s="8"/>
       <c r="F159" s="8"/>
       <c r="G159" s="8"/>
-      <c r="O159" s="3"/>
-      <c r="P159" s="3"/>
-    </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W159" s="3"/>
+      <c r="X159" s="3"/>
+    </row>
+    <row r="160" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="8"/>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
@@ -5936,10 +6051,10 @@
       <c r="E160" s="8"/>
       <c r="F160" s="8"/>
       <c r="G160" s="8"/>
-      <c r="O160" s="3"/>
-      <c r="P160" s="3"/>
-    </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W160" s="3"/>
+      <c r="X160" s="3"/>
+    </row>
+    <row r="161" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="8"/>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
@@ -5947,10 +6062,10 @@
       <c r="E161" s="8"/>
       <c r="F161" s="8"/>
       <c r="G161" s="8"/>
-      <c r="O161" s="3"/>
-      <c r="P161" s="3"/>
-    </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W161" s="3"/>
+      <c r="X161" s="3"/>
+    </row>
+    <row r="162" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
@@ -5958,10 +6073,10 @@
       <c r="E162" s="8"/>
       <c r="F162" s="8"/>
       <c r="G162" s="8"/>
-      <c r="O162" s="3"/>
-      <c r="P162" s="3"/>
-    </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W162" s="3"/>
+      <c r="X162" s="3"/>
+    </row>
+    <row r="163" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="8"/>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
@@ -5969,10 +6084,10 @@
       <c r="E163" s="8"/>
       <c r="F163" s="8"/>
       <c r="G163" s="8"/>
-      <c r="O163" s="3"/>
-      <c r="P163" s="3"/>
-    </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W163" s="3"/>
+      <c r="X163" s="3"/>
+    </row>
+    <row r="164" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="8"/>
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
@@ -5980,10 +6095,10 @@
       <c r="E164" s="8"/>
       <c r="F164" s="8"/>
       <c r="G164" s="8"/>
-      <c r="O164" s="3"/>
-      <c r="P164" s="3"/>
-    </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W164" s="3"/>
+      <c r="X164" s="3"/>
+    </row>
+    <row r="165" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="8"/>
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
@@ -5991,10 +6106,10 @@
       <c r="E165" s="8"/>
       <c r="F165" s="8"/>
       <c r="G165" s="8"/>
-      <c r="O165" s="3"/>
-      <c r="P165" s="3"/>
-    </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W165" s="3"/>
+      <c r="X165" s="3"/>
+    </row>
+    <row r="166" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="8"/>
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
@@ -6002,10 +6117,10 @@
       <c r="E166" s="8"/>
       <c r="F166" s="8"/>
       <c r="G166" s="8"/>
-      <c r="O166" s="3"/>
-      <c r="P166" s="3"/>
-    </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W166" s="3"/>
+      <c r="X166" s="3"/>
+    </row>
+    <row r="167" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="8"/>
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
@@ -6013,10 +6128,10 @@
       <c r="E167" s="8"/>
       <c r="F167" s="8"/>
       <c r="G167" s="8"/>
-      <c r="O167" s="3"/>
-      <c r="P167" s="3"/>
-    </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W167" s="3"/>
+      <c r="X167" s="3"/>
+    </row>
+    <row r="168" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="8"/>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
@@ -6024,10 +6139,10 @@
       <c r="E168" s="8"/>
       <c r="F168" s="8"/>
       <c r="G168" s="8"/>
-      <c r="O168" s="3"/>
-      <c r="P168" s="3"/>
-    </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W168" s="3"/>
+      <c r="X168" s="3"/>
+    </row>
+    <row r="169" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="8"/>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
@@ -6035,10 +6150,10 @@
       <c r="E169" s="8"/>
       <c r="F169" s="8"/>
       <c r="G169" s="8"/>
-      <c r="O169" s="3"/>
-      <c r="P169" s="3"/>
-    </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W169" s="3"/>
+      <c r="X169" s="3"/>
+    </row>
+    <row r="170" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="8"/>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
@@ -6046,10 +6161,10 @@
       <c r="E170" s="8"/>
       <c r="F170" s="8"/>
       <c r="G170" s="8"/>
-      <c r="O170" s="3"/>
-      <c r="P170" s="3"/>
-    </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W170" s="3"/>
+      <c r="X170" s="3"/>
+    </row>
+    <row r="171" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="8"/>
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
@@ -6057,10 +6172,10 @@
       <c r="E171" s="8"/>
       <c r="F171" s="8"/>
       <c r="G171" s="8"/>
-      <c r="O171" s="3"/>
-      <c r="P171" s="3"/>
-    </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W171" s="3"/>
+      <c r="X171" s="3"/>
+    </row>
+    <row r="172" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="8"/>
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
@@ -6068,10 +6183,10 @@
       <c r="E172" s="8"/>
       <c r="F172" s="8"/>
       <c r="G172" s="8"/>
-      <c r="O172" s="3"/>
-      <c r="P172" s="3"/>
-    </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W172" s="3"/>
+      <c r="X172" s="3"/>
+    </row>
+    <row r="173" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="8"/>
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
@@ -6079,10 +6194,10 @@
       <c r="E173" s="8"/>
       <c r="F173" s="8"/>
       <c r="G173" s="8"/>
-      <c r="O173" s="3"/>
-      <c r="P173" s="3"/>
-    </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W173" s="3"/>
+      <c r="X173" s="3"/>
+    </row>
+    <row r="174" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="8"/>
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
@@ -6090,10 +6205,10 @@
       <c r="E174" s="8"/>
       <c r="F174" s="8"/>
       <c r="G174" s="8"/>
-      <c r="O174" s="3"/>
-      <c r="P174" s="3"/>
-    </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W174" s="3"/>
+      <c r="X174" s="3"/>
+    </row>
+    <row r="175" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="8"/>
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
@@ -6101,10 +6216,10 @@
       <c r="E175" s="8"/>
       <c r="F175" s="8"/>
       <c r="G175" s="8"/>
-      <c r="O175" s="3"/>
-      <c r="P175" s="3"/>
-    </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W175" s="3"/>
+      <c r="X175" s="3"/>
+    </row>
+    <row r="176" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="8"/>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
@@ -6112,10 +6227,10 @@
       <c r="E176" s="8"/>
       <c r="F176" s="8"/>
       <c r="G176" s="8"/>
-      <c r="O176" s="3"/>
-      <c r="P176" s="3"/>
-    </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W176" s="3"/>
+      <c r="X176" s="3"/>
+    </row>
+    <row r="177" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="8"/>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
@@ -6123,10 +6238,10 @@
       <c r="E177" s="8"/>
       <c r="F177" s="8"/>
       <c r="G177" s="8"/>
-      <c r="O177" s="3"/>
-      <c r="P177" s="3"/>
-    </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W177" s="3"/>
+      <c r="X177" s="3"/>
+    </row>
+    <row r="178" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
@@ -6134,10 +6249,10 @@
       <c r="E178" s="8"/>
       <c r="F178" s="8"/>
       <c r="G178" s="8"/>
-      <c r="O178" s="3"/>
-      <c r="P178" s="3"/>
-    </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W178" s="3"/>
+      <c r="X178" s="3"/>
+    </row>
+    <row r="179" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="8"/>
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
@@ -6145,10 +6260,10 @@
       <c r="E179" s="8"/>
       <c r="F179" s="8"/>
       <c r="G179" s="8"/>
-      <c r="O179" s="3"/>
-      <c r="P179" s="3"/>
-    </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W179" s="3"/>
+      <c r="X179" s="3"/>
+    </row>
+    <row r="180" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="8"/>
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
@@ -6156,10 +6271,10 @@
       <c r="E180" s="8"/>
       <c r="F180" s="8"/>
       <c r="G180" s="8"/>
-      <c r="O180" s="3"/>
-      <c r="P180" s="3"/>
-    </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W180" s="3"/>
+      <c r="X180" s="3"/>
+    </row>
+    <row r="181" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="8"/>
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
@@ -6167,10 +6282,10 @@
       <c r="E181" s="8"/>
       <c r="F181" s="8"/>
       <c r="G181" s="8"/>
-      <c r="O181" s="3"/>
-      <c r="P181" s="3"/>
-    </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W181" s="3"/>
+      <c r="X181" s="3"/>
+    </row>
+    <row r="182" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
@@ -6178,10 +6293,10 @@
       <c r="E182" s="8"/>
       <c r="F182" s="8"/>
       <c r="G182" s="8"/>
-      <c r="O182" s="3"/>
-      <c r="P182" s="3"/>
-    </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W182" s="3"/>
+      <c r="X182" s="3"/>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
@@ -6189,10 +6304,10 @@
       <c r="E183" s="8"/>
       <c r="F183" s="8"/>
       <c r="G183" s="8"/>
-      <c r="O183" s="3"/>
-      <c r="P183" s="3"/>
-    </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W183" s="3"/>
+      <c r="X183" s="3"/>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
@@ -6200,10 +6315,10 @@
       <c r="E184" s="8"/>
       <c r="F184" s="8"/>
       <c r="G184" s="8"/>
-      <c r="O184" s="3"/>
-      <c r="P184" s="3"/>
-    </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W184" s="3"/>
+      <c r="X184" s="3"/>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="8"/>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
@@ -6211,10 +6326,10 @@
       <c r="E185" s="8"/>
       <c r="F185" s="8"/>
       <c r="G185" s="8"/>
-      <c r="O185" s="3"/>
-      <c r="P185" s="3"/>
-    </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W185" s="3"/>
+      <c r="X185" s="3"/>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
@@ -6222,10 +6337,10 @@
       <c r="E186" s="8"/>
       <c r="F186" s="8"/>
       <c r="G186" s="8"/>
-      <c r="O186" s="3"/>
-      <c r="P186" s="3"/>
-    </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W186" s="3"/>
+      <c r="X186" s="3"/>
+    </row>
+    <row r="187" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
@@ -6233,10 +6348,10 @@
       <c r="E187" s="8"/>
       <c r="F187" s="8"/>
       <c r="G187" s="8"/>
-      <c r="O187" s="3"/>
-      <c r="P187" s="3"/>
-    </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W187" s="3"/>
+      <c r="X187" s="3"/>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
@@ -6244,10 +6359,10 @@
       <c r="E188" s="8"/>
       <c r="F188" s="8"/>
       <c r="G188" s="8"/>
-      <c r="O188" s="3"/>
-      <c r="P188" s="3"/>
-    </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W188" s="3"/>
+      <c r="X188" s="3"/>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
@@ -6255,10 +6370,10 @@
       <c r="E189" s="8"/>
       <c r="F189" s="8"/>
       <c r="G189" s="8"/>
-      <c r="O189" s="3"/>
-      <c r="P189" s="3"/>
-    </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W189" s="3"/>
+      <c r="X189" s="3"/>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="8"/>
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
@@ -6266,10 +6381,10 @@
       <c r="E190" s="8"/>
       <c r="F190" s="8"/>
       <c r="G190" s="8"/>
-      <c r="O190" s="3"/>
-      <c r="P190" s="3"/>
-    </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W190" s="3"/>
+      <c r="X190" s="3"/>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="8"/>
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
@@ -6277,10 +6392,10 @@
       <c r="E191" s="8"/>
       <c r="F191" s="8"/>
       <c r="G191" s="8"/>
-      <c r="O191" s="3"/>
-      <c r="P191" s="3"/>
-    </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W191" s="3"/>
+      <c r="X191" s="3"/>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="8"/>
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
@@ -6288,10 +6403,10 @@
       <c r="E192" s="8"/>
       <c r="F192" s="8"/>
       <c r="G192" s="8"/>
-      <c r="O192" s="3"/>
-      <c r="P192" s="3"/>
-    </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W192" s="3"/>
+      <c r="X192" s="3"/>
+    </row>
+    <row r="193" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
@@ -6299,10 +6414,10 @@
       <c r="E193" s="8"/>
       <c r="F193" s="8"/>
       <c r="G193" s="8"/>
-      <c r="O193" s="3"/>
-      <c r="P193" s="3"/>
-    </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W193" s="3"/>
+      <c r="X193" s="3"/>
+    </row>
+    <row r="194" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
@@ -6310,10 +6425,10 @@
       <c r="E194" s="8"/>
       <c r="F194" s="8"/>
       <c r="G194" s="8"/>
-      <c r="O194" s="3"/>
-      <c r="P194" s="3"/>
-    </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W194" s="3"/>
+      <c r="X194" s="3"/>
+    </row>
+    <row r="195" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="8"/>
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
@@ -6321,10 +6436,10 @@
       <c r="E195" s="8"/>
       <c r="F195" s="8"/>
       <c r="G195" s="8"/>
-      <c r="O195" s="3"/>
-      <c r="P195" s="3"/>
-    </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W195" s="3"/>
+      <c r="X195" s="3"/>
+    </row>
+    <row r="196" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
@@ -6332,10 +6447,10 @@
       <c r="E196" s="8"/>
       <c r="F196" s="8"/>
       <c r="G196" s="8"/>
-      <c r="O196" s="3"/>
-      <c r="P196" s="3"/>
-    </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W196" s="3"/>
+      <c r="X196" s="3"/>
+    </row>
+    <row r="197" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="8"/>
       <c r="B197" s="8"/>
       <c r="C197" s="8"/>
@@ -6343,10 +6458,10 @@
       <c r="E197" s="8"/>
       <c r="F197" s="8"/>
       <c r="G197" s="8"/>
-      <c r="O197" s="3"/>
-      <c r="P197" s="3"/>
-    </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W197" s="3"/>
+      <c r="X197" s="3"/>
+    </row>
+    <row r="198" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="8"/>
       <c r="B198" s="8"/>
       <c r="C198" s="8"/>
@@ -6354,10 +6469,10 @@
       <c r="E198" s="8"/>
       <c r="F198" s="8"/>
       <c r="G198" s="8"/>
-      <c r="O198" s="3"/>
-      <c r="P198" s="3"/>
-    </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W198" s="3"/>
+      <c r="X198" s="3"/>
+    </row>
+    <row r="199" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
@@ -6365,10 +6480,10 @@
       <c r="E199" s="8"/>
       <c r="F199" s="8"/>
       <c r="G199" s="8"/>
-      <c r="O199" s="21"/>
-      <c r="P199" s="21"/>
-    </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W199" s="21"/>
+      <c r="X199" s="21"/>
+    </row>
+    <row r="200" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="8"/>
       <c r="B200" s="8"/>
       <c r="C200" s="8"/>
@@ -6376,10 +6491,10 @@
       <c r="E200" s="8"/>
       <c r="F200" s="8"/>
       <c r="G200" s="9"/>
-      <c r="O200" s="3"/>
-      <c r="P200" s="3"/>
-    </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="W200" s="3"/>
+      <c r="X200" s="3"/>
+    </row>
+    <row r="201" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="10"/>
       <c r="B201" s="10"/>
       <c r="C201" s="10"/>
@@ -6387,20 +6502,27 @@
       <c r="E201" s="10"/>
       <c r="F201" s="10"/>
       <c r="G201" s="11"/>
-      <c r="O201" s="3"/>
-      <c r="P201" s="3"/>
+      <c r="W201" s="3"/>
+      <c r="X201" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="無効なID" error="IDは0より大きい整数である必要があります。" sqref="O2:O1048576" xr:uid="{8ED4B105-B57E-483A-A8E7-5AD93587E784}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:K1048576 N2:N1048576 U2:V1048576 P2:Q1048576" xr:uid="{C260899B-113D-470B-89F6-D6A3946916A9}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="無効なID" error="IDは0より大きい整数である必要があります。" sqref="W2:W1048576" xr:uid="{8ED4B105-B57E-483A-A8E7-5AD93587E784}">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:K1048576 N2:N1048576" xr:uid="{C260899B-113D-470B-89F6-D6A3946916A9}">
-      <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{D95B43DE-6095-484D-B17C-048FD7035870}">
       <formula1>"NonProduction, Attended, Unattended, Studio, Development, StudioX, Headless, StudioPro, TestAutomation"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:T1048576" xr:uid="{5325A3FF-07E7-4CA1-A4A0-D0CC08FC1CA1}">
+      <formula1>0</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{F6B5ED4E-5129-4EEA-8960-EA4924F56786}">
+      <formula1>"Verbose, Trace, Information, Warning, Error, Critical, Off"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve Edit User to accept AR/UR settings
</commit_message>
<xml_diff>
--- a/Workbooks/JA/ユーザー.xlsx
+++ b/Workbooks/JA/ユーザー.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABC55F9-43C9-4F4B-8946-A46B5D82C96D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500106A1-4D45-4507-A11C-FEB391C3512E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="4940" windowWidth="30570" windowHeight="11930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58695" yWindow="1005" windowWidth="26580" windowHeight="12930" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>名</t>
   </si>
@@ -519,30 +519,171 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="82">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1043,6 +1184,30 @@
         </bottom>
       </border>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1580,105 +1745,120 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="66" dataDxfId="64" totalsRowDxfId="62" headerRowBorderDxfId="65" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:I201" headerRowDxfId="81" dataDxfId="79" totalsRowDxfId="77" headerRowBorderDxfId="80" tableBorderDxfId="78">
   <autoFilter ref="A1:I201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{C22893F0-4B4D-460C-A013-95020C7502B4}" name="タイプ" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{1372863E-1574-486C-96A5-9F8A48DBEB17}" name="ID" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="ユーザー名" dataDxfId="58"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="名" totalsRowLabel="Total" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="姓" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="メールアドレス" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="組織単位名" totalsRowFunction="count" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="ロール名" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{73F4371D-09E6-432B-A8D2-FDF51584A3F9}" name="ステータス" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{C22893F0-4B4D-460C-A013-95020C7502B4}" name="タイプ" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{1372863E-1574-486C-96A5-9F8A48DBEB17}" name="ID" dataDxfId="74"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="ユーザー名" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="名" totalsRowLabel="Total" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="姓" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="メールアドレス" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="組織単位名" totalsRowFunction="count" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="ロール名" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{73F4371D-09E6-432B-A8D2-FDF51584A3F9}" name="ステータス" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:X201" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:X201" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A1:X201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="24">
-    <tableColumn id="10" xr3:uid="{65749B7E-1278-4BF9-BE0E-B0B1A7EBF445}" name="ユーザー名 *" dataDxfId="49"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="名" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="姓" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="メールアドレス" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="組織単位名" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="ロール" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{4E111FFE-AC48-4FF2-B3E5-DEDE4EC1D531}" name="パスワード" dataDxfId="43"/>
-    <tableColumn id="14" xr3:uid="{6DE9A60B-D2AA-4C5B-9D19-151C1E73E0AC}" name="ドメイン\ユーザ名 - Attended ロボット" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{262304B2-69B6-47FC-833F-5922ED105520}" name="ライセンスの種類 - Attended ロボット" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{42564DA4-8D53-4C1B-9C2C-4BE92DD00FFC}" name="個人のワークスペースを作成 - Attended ロボット" dataDxfId="40"/>
-    <tableColumn id="16" xr3:uid="{49DD615B-15C2-4B9A-960E-9A70F1B8C51E}" name="スタンドアロンライセンス - Attended ロボット" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{B5515926-7E95-4BDC-B434-092F68C9E676}" name="ドメイン\ユーザー名 - Unattended ロボット" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{1EFF2166-C43F-4EFE-A90C-FFD898ED903B}" name="パスワード - Unattended Robot" dataDxfId="37"/>
-    <tableColumn id="17" xr3:uid="{E40F7CE9-454E-4944-9C0F-78161314E5AC}" name="同時接続実行を無効化 - Unattended Robot" dataDxfId="36"/>
-    <tableColumn id="24" xr3:uid="{4737097B-807F-467E-994B-823169C8851E}" name="ログレベル" dataDxfId="7"/>
-    <tableColumn id="23" xr3:uid="{F4F5E00E-44D5-478B-9E16-1E0836A97A31}" name="開発ログを許可" dataDxfId="6"/>
-    <tableColumn id="22" xr3:uid="{54CE7D6A-8149-4FF1-856C-0297F6C4EA6A}" name="コンソールへログイン" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{981701E3-426C-4D88-A3C1-45F9E3D28795}" name="解像度の幅" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{9DC42AD1-736C-4BEB-A7A8-35E20A7368C1}" name="解像度の高さ" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{45F1E31B-C2C4-4911-8745-575C838381F3}" name="解像度の階調" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{433CEED5-AD86-4341-87B3-24E355BD37E2}" name="フォントスムージング" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{ABE2AD9D-F7D1-4BD9-B771-C5E569C50B19}" name="プロセスを自動ダウンロード" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="ID" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{08B4DCAC-6628-4928-B533-CE43508622D2}" name="結果" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{65749B7E-1278-4BF9-BE0E-B0B1A7EBF445}" name="ユーザー名 *" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="名" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="姓" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="メールアドレス" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="組織単位名" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{42F54A22-BA7B-4DC3-BF4D-BA0546417160}" name="ロール" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{4E111FFE-AC48-4FF2-B3E5-DEDE4EC1D531}" name="パスワード" dataDxfId="58"/>
+    <tableColumn id="14" xr3:uid="{6DE9A60B-D2AA-4C5B-9D19-151C1E73E0AC}" name="ドメイン\ユーザ名 - Attended ロボット" dataDxfId="57"/>
+    <tableColumn id="13" xr3:uid="{262304B2-69B6-47FC-833F-5922ED105520}" name="ライセンスの種類 - Attended ロボット" dataDxfId="56"/>
+    <tableColumn id="15" xr3:uid="{42564DA4-8D53-4C1B-9C2C-4BE92DD00FFC}" name="個人のワークスペースを作成 - Attended ロボット" dataDxfId="55"/>
+    <tableColumn id="16" xr3:uid="{49DD615B-15C2-4B9A-960E-9A70F1B8C51E}" name="スタンドアロンライセンス - Attended ロボット" dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{B5515926-7E95-4BDC-B434-092F68C9E676}" name="ドメイン\ユーザー名 - Unattended ロボット" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{1EFF2166-C43F-4EFE-A90C-FFD898ED903B}" name="パスワード - Unattended Robot" dataDxfId="52"/>
+    <tableColumn id="17" xr3:uid="{E40F7CE9-454E-4944-9C0F-78161314E5AC}" name="同時接続実行を無効化 - Unattended Robot" dataDxfId="51"/>
+    <tableColumn id="24" xr3:uid="{4737097B-807F-467E-994B-823169C8851E}" name="ログレベル" dataDxfId="50"/>
+    <tableColumn id="23" xr3:uid="{F4F5E00E-44D5-478B-9E16-1E0836A97A31}" name="開発ログを許可" dataDxfId="49"/>
+    <tableColumn id="22" xr3:uid="{54CE7D6A-8149-4FF1-856C-0297F6C4EA6A}" name="コンソールへログイン" dataDxfId="48"/>
+    <tableColumn id="21" xr3:uid="{981701E3-426C-4D88-A3C1-45F9E3D28795}" name="解像度の幅" dataDxfId="47"/>
+    <tableColumn id="20" xr3:uid="{9DC42AD1-736C-4BEB-A7A8-35E20A7368C1}" name="解像度の高さ" dataDxfId="46"/>
+    <tableColumn id="19" xr3:uid="{45F1E31B-C2C4-4911-8745-575C838381F3}" name="解像度の階調" dataDxfId="45"/>
+    <tableColumn id="18" xr3:uid="{433CEED5-AD86-4341-87B3-24E355BD37E2}" name="フォントスムージング" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{ABE2AD9D-F7D1-4BD9-B771-C5E569C50B19}" name="プロセスを自動ダウンロード" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{E2F843A0-E163-4591-A90A-DA03F637285C}" name="ID" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{08B4DCAC-6628-4928-B533-CE43508622D2}" name="結果" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:G201" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="A1:G201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{01450210-36BE-4B28-9B3B-758A2770B142}" name="ID" dataDxfId="31"/>
-    <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="名" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="姓" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="メールアドレス" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{310BA8C6-70B4-40F4-B90F-2C40BB19BC10}" name="ステータス" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="パスワード" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{E7804193-086E-4884-9B07-86C7E77E0835}" name="結果" dataDxfId="25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40330C-E043-47F5-9A1D-98C4F5DCAE20}" name="Table15" displayName="Table15" ref="A1:V201" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:V201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="22">
+    <tableColumn id="3" xr3:uid="{01450210-36BE-4B28-9B3B-758A2770B142}" name="ID" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{D002318D-F09E-4941-86F7-CB540B53CA38}" name="名" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{A5B9750D-9F4C-4ACD-B998-452D86A89786}" name="姓" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{FB9ABF1E-6D2B-4148-9C75-B26D470A604D}" name="メールアドレス" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{310BA8C6-70B4-40F4-B90F-2C40BB19BC10}" name="ステータス" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{34576645-A498-4AA2-BA38-3776D490DE1A}" name="パスワード" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{0A9FCE5D-7A4D-4D23-962D-3D890B31ECF6}" name="ドメイン\ユーザ名 - Attended ロボット" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{435EC5F0-D9A6-492E-AFC0-0DF64431D694}" name="ライセンスの種類 - Attended ロボット" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{78B66692-FDB2-4164-9EF9-EF729C4B3EE1}" name="個人のワークスペースを作成 - Attended ロボット" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{D39B748A-CEBA-4449-9A1E-C1A802A5B8E3}" name="スタンドアロンライセンス - Attended ロボット" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{E8BC110B-0EF0-4150-9004-8FD287FCEF10}" name="ドメイン\ユーザー名 - Unattended ロボット" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{C8D99A10-4E3F-4431-93D3-322E7C3CB822}" name="パスワード - Unattended Robot" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{D2D0C529-C8B4-4DAF-A87D-78D50327198E}" name="同時接続実行を無効化 - Unattended Robot" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{38F4D0BE-C738-4ED6-8F58-D9C863FB5182}" name="ログレベル" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{CA205852-D1C8-420F-9E61-81D5982308DE}" name="開発ログを許可" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{79F01462-F7AD-4A8F-8909-36D6802C36D3}" name="コンソールへログイン" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{503CA7D4-BC2E-4C6E-AE61-92987D0598E5}" name="解像度の幅" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{3A8786A2-3903-4EC9-90F0-3A1636A30463}" name="解像度の高さ" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{F7A5386B-EFAF-44D1-8380-825CDA61BD20}" name="解像度の階調" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{A1080AA5-CC3A-43C6-B6E2-8A15B9C71902}" name="フォントスムージング" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{B72276C2-2DF1-4464-97AF-8B980AA55BC1}" name="プロセスを自動ダウンロード" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{E7804193-086E-4884-9B07-86C7E77E0835}" name="結果" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C201" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C201" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:C201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID" dataDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ユーザー名" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="結果" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ユーザー名" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{789EC9DB-B69B-4343-B58A-CF450EDB59BF}" name="結果" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9A9C6F0D-2E14-43CF-BA3F-71838E8A8593}" name="Table1367" displayName="Table1367" ref="A1:D201" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9A9C6F0D-2E14-43CF-BA3F-71838E8A8593}" name="Table1367" displayName="Table1367" ref="A1:D201" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EB9188D5-49DF-4F54-A843-A55D3E2C1BE7}" name="ユーザー ID" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{85E99034-1CC5-49C9-990E-916A8CEEC70B}" name="追加されるロール名" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{CE37118B-AB12-42D8-BD3F-A9948E262C56}" name="削除されるロール名" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{C8060084-F897-4904-AA9C-11EEA24740A4}" name="結果" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{EB9188D5-49DF-4F54-A843-A55D3E2C1BE7}" name="ユーザー ID" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{85E99034-1CC5-49C9-990E-916A8CEEC70B}" name="追加されるロール名" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{CE37118B-AB12-42D8-BD3F-A9948E262C56}" name="削除されるロール名" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{C8060084-F897-4904-AA9C-11EEA24740A4}" name="結果" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F4943553-1107-4ABF-92F1-3D44259ECE3F}" name="Table136" displayName="Table136" ref="A1:D201" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F4943553-1107-4ABF-92F1-3D44259ECE3F}" name="Table136" displayName="Table136" ref="A1:D201" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AECF12CD-DED5-4EAC-990D-027FA15BD77B}" name="ユーザーID" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{386847AF-7B54-40AC-B632-9092A64C412D}" name="追加される組織単位名" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{927EBCB0-231E-4AA5-99D9-8C13EE557A37}" name="削除される組織単位名" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{85CBEB5B-343A-4F2F-8DE9-C961C7CE168C}" name="結果" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{AECF12CD-DED5-4EAC-990D-027FA15BD77B}" name="ユーザーID" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{386847AF-7B54-40AC-B632-9092A64C412D}" name="追加される組織単位名" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{927EBCB0-231E-4AA5-99D9-8C13EE557A37}" name="削除される組織単位名" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{85CBEB5B-343A-4F2F-8DE9-C961C7CE168C}" name="結果" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4214,8 +4394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V1" sqref="H1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -6535,23 +6715,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF20293-3040-451C-BEA0-1DF5FCF14B01}">
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:V201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
-    <col min="2" max="4" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="45.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.75" style="2"/>
+    <col min="1" max="1" width="15.6640625" style="29" customWidth="1"/>
+    <col min="2" max="4" width="25.6640625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="29" customWidth="1"/>
+    <col min="7" max="13" width="25.5" style="2" customWidth="1"/>
+    <col min="14" max="21" width="25.75" style="2" customWidth="1"/>
+    <col min="22" max="22" width="45.6640625" style="31" customWidth="1"/>
+    <col min="23" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:22" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -6570,1818 +6752,1876 @@
       <c r="F1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="12"/>
       <c r="F2" s="25"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="12"/>
       <c r="F3" s="25"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V3" s="3"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="12"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V4" s="3"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="12"/>
       <c r="F5" s="25"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="12"/>
       <c r="F6" s="25"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="12"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="12"/>
       <c r="F8" s="25"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="12"/>
       <c r="F9" s="25"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V9" s="3"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="12"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="12"/>
       <c r="F10" s="25"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V10" s="3"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V11" s="3"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V12" s="3"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V13" s="3"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V16" s="3"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V17" s="3"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V18" s="3"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V19" s="3"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V20" s="3"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V21" s="3"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V22" s="3"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V23" s="3"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V24" s="3"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V25" s="3"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V26" s="3"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V27" s="3"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V28" s="3"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V29" s="3"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V30" s="3"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V31" s="3"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V32" s="3"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V33" s="3"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V34" s="3"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V35" s="3"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V36" s="3"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V37" s="3"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V38" s="3"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V39" s="3"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V40" s="3"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V41" s="3"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V42" s="3"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V43" s="3"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V44" s="3"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V45" s="3"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V46" s="3"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="9"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V47" s="3"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V48" s="3"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V49" s="3"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V50" s="3"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V51" s="3"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V52" s="3"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V53" s="3"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V54" s="3"/>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="3"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V55" s="3"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="3"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V56" s="3"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="3"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V57" s="3"/>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V58" s="3"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="3"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V59" s="3"/>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="3"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V60" s="3"/>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="9"/>
-      <c r="G61" s="3"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V61" s="3"/>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
       <c r="F62" s="9"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V62" s="3"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V63" s="3"/>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="3"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V64" s="3"/>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="3"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V65" s="3"/>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="3"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V66" s="3"/>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="3"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V67" s="3"/>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
       <c r="F68" s="9"/>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V68" s="3"/>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
       <c r="F69" s="9"/>
-      <c r="G69" s="3"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V69" s="3"/>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
       <c r="F70" s="9"/>
-      <c r="G70" s="3"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V70" s="3"/>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
       <c r="F71" s="9"/>
-      <c r="G71" s="3"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V71" s="3"/>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
       <c r="F72" s="9"/>
-      <c r="G72" s="3"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V72" s="3"/>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
       <c r="F73" s="9"/>
-      <c r="G73" s="3"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V73" s="3"/>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="9"/>
-      <c r="G74" s="3"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V74" s="3"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="9"/>
-      <c r="G75" s="3"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V75" s="3"/>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
       <c r="F76" s="9"/>
-      <c r="G76" s="3"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V76" s="3"/>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
       <c r="F77" s="9"/>
-      <c r="G77" s="3"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V77" s="3"/>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
       <c r="F78" s="9"/>
-      <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V78" s="3"/>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
       <c r="F79" s="9"/>
-      <c r="G79" s="3"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V79" s="3"/>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
       <c r="F80" s="9"/>
-      <c r="G80" s="3"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V80" s="3"/>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8"/>
       <c r="F81" s="9"/>
-      <c r="G81" s="3"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V81" s="3"/>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
       <c r="F82" s="9"/>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V82" s="3"/>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
       <c r="F83" s="9"/>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V83" s="3"/>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
       <c r="F84" s="9"/>
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V84" s="3"/>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
       <c r="F85" s="9"/>
-      <c r="G85" s="3"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V85" s="3"/>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
       <c r="F86" s="9"/>
-      <c r="G86" s="3"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V86" s="3"/>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
       <c r="F87" s="9"/>
-      <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V87" s="3"/>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
       <c r="F88" s="9"/>
-      <c r="G88" s="3"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V88" s="3"/>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
       <c r="F89" s="9"/>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V89" s="3"/>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
       <c r="F90" s="9"/>
-      <c r="G90" s="3"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V90" s="3"/>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
       <c r="F91" s="9"/>
-      <c r="G91" s="3"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V91" s="3"/>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
       <c r="F92" s="9"/>
-      <c r="G92" s="3"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V92" s="3"/>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
       <c r="F93" s="9"/>
-      <c r="G93" s="3"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V93" s="3"/>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
       <c r="F94" s="9"/>
-      <c r="G94" s="3"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V94" s="3"/>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
       <c r="F95" s="9"/>
-      <c r="G95" s="3"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V95" s="3"/>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
       <c r="F96" s="9"/>
-      <c r="G96" s="3"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V96" s="3"/>
+    </row>
+    <row r="97" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
       <c r="F97" s="9"/>
-      <c r="G97" s="3"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V97" s="3"/>
+    </row>
+    <row r="98" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
       <c r="F98" s="9"/>
-      <c r="G98" s="3"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V98" s="3"/>
+    </row>
+    <row r="99" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
       <c r="F99" s="9"/>
-      <c r="G99" s="3"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V99" s="3"/>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
       <c r="E100" s="8"/>
       <c r="F100" s="9"/>
-      <c r="G100" s="3"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V100" s="3"/>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="8"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
       <c r="F101" s="9"/>
-      <c r="G101" s="3"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V101" s="3"/>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
       <c r="E102" s="8"/>
       <c r="F102" s="8"/>
-      <c r="G102" s="3"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V102" s="3"/>
+    </row>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
       <c r="E103" s="8"/>
       <c r="F103" s="8"/>
-      <c r="G103" s="3"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V103" s="3"/>
+    </row>
+    <row r="104" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
       <c r="E104" s="8"/>
       <c r="F104" s="8"/>
-      <c r="G104" s="3"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V104" s="3"/>
+    </row>
+    <row r="105" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
       <c r="F105" s="8"/>
-      <c r="G105" s="3"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V105" s="3"/>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="8"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
       <c r="F106" s="8"/>
-      <c r="G106" s="3"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V106" s="3"/>
+    </row>
+    <row r="107" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="8"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
       <c r="E107" s="8"/>
       <c r="F107" s="8"/>
-      <c r="G107" s="3"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V107" s="3"/>
+    </row>
+    <row r="108" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
-      <c r="G108" s="3"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V108" s="3"/>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
       <c r="F109" s="8"/>
-      <c r="G109" s="3"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V109" s="3"/>
+    </row>
+    <row r="110" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
       <c r="E110" s="8"/>
       <c r="F110" s="8"/>
-      <c r="G110" s="3"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V110" s="3"/>
+    </row>
+    <row r="111" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
-      <c r="G111" s="3"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V111" s="3"/>
+    </row>
+    <row r="112" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
       <c r="E112" s="8"/>
       <c r="F112" s="8"/>
-      <c r="G112" s="3"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V112" s="3"/>
+    </row>
+    <row r="113" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
-      <c r="G113" s="3"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V113" s="3"/>
+    </row>
+    <row r="114" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="8"/>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
       <c r="E114" s="8"/>
       <c r="F114" s="8"/>
-      <c r="G114" s="3"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V114" s="3"/>
+    </row>
+    <row r="115" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="8"/>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
-      <c r="G115" s="3"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V115" s="3"/>
+    </row>
+    <row r="116" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
-      <c r="G116" s="3"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V116" s="3"/>
+    </row>
+    <row r="117" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="8"/>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
-      <c r="G117" s="3"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V117" s="3"/>
+    </row>
+    <row r="118" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
-      <c r="G118" s="3"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V118" s="3"/>
+    </row>
+    <row r="119" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
-      <c r="G119" s="3"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V119" s="3"/>
+    </row>
+    <row r="120" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="8"/>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
-      <c r="G120" s="3"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V120" s="3"/>
+    </row>
+    <row r="121" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="8"/>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
-      <c r="G121" s="3"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V121" s="3"/>
+    </row>
+    <row r="122" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
-      <c r="G122" s="3"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V122" s="3"/>
+    </row>
+    <row r="123" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
-      <c r="G123" s="3"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V123" s="3"/>
+    </row>
+    <row r="124" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
-      <c r="G124" s="3"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V124" s="3"/>
+    </row>
+    <row r="125" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="8"/>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
-      <c r="G125" s="3"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V125" s="3"/>
+    </row>
+    <row r="126" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="8"/>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
-      <c r="G126" s="3"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V126" s="3"/>
+    </row>
+    <row r="127" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="8"/>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
       <c r="F127" s="8"/>
-      <c r="G127" s="3"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V127" s="3"/>
+    </row>
+    <row r="128" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="8"/>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
       <c r="E128" s="8"/>
       <c r="F128" s="8"/>
-      <c r="G128" s="3"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V128" s="3"/>
+    </row>
+    <row r="129" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="8"/>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
       <c r="E129" s="8"/>
       <c r="F129" s="8"/>
-      <c r="G129" s="3"/>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V129" s="3"/>
+    </row>
+    <row r="130" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="8"/>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
       <c r="E130" s="8"/>
       <c r="F130" s="8"/>
-      <c r="G130" s="3"/>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V130" s="3"/>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="8"/>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
       <c r="E131" s="8"/>
       <c r="F131" s="8"/>
-      <c r="G131" s="3"/>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V131" s="3"/>
+    </row>
+    <row r="132" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="8"/>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
       <c r="E132" s="8"/>
       <c r="F132" s="8"/>
-      <c r="G132" s="3"/>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V132" s="3"/>
+    </row>
+    <row r="133" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="8"/>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
       <c r="E133" s="8"/>
       <c r="F133" s="8"/>
-      <c r="G133" s="3"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V133" s="3"/>
+    </row>
+    <row r="134" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="8"/>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
       <c r="E134" s="8"/>
       <c r="F134" s="8"/>
-      <c r="G134" s="3"/>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V134" s="3"/>
+    </row>
+    <row r="135" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="8"/>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
       <c r="E135" s="8"/>
       <c r="F135" s="8"/>
-      <c r="G135" s="3"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V135" s="3"/>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
       <c r="F136" s="8"/>
-      <c r="G136" s="3"/>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V136" s="3"/>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="8"/>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
       <c r="E137" s="8"/>
       <c r="F137" s="8"/>
-      <c r="G137" s="3"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V137" s="3"/>
+    </row>
+    <row r="138" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
       <c r="E138" s="8"/>
       <c r="F138" s="8"/>
-      <c r="G138" s="3"/>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V138" s="3"/>
+    </row>
+    <row r="139" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="8"/>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
       <c r="E139" s="8"/>
       <c r="F139" s="8"/>
-      <c r="G139" s="3"/>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V139" s="3"/>
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="8"/>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
       <c r="E140" s="8"/>
       <c r="F140" s="8"/>
-      <c r="G140" s="3"/>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V140" s="3"/>
+    </row>
+    <row r="141" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="8"/>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
       <c r="E141" s="8"/>
       <c r="F141" s="8"/>
-      <c r="G141" s="3"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V141" s="3"/>
+    </row>
+    <row r="142" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
       <c r="F142" s="8"/>
-      <c r="G142" s="3"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V142" s="3"/>
+    </row>
+    <row r="143" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
       <c r="E143" s="8"/>
       <c r="F143" s="8"/>
-      <c r="G143" s="3"/>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V143" s="3"/>
+    </row>
+    <row r="144" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
       <c r="E144" s="8"/>
       <c r="F144" s="8"/>
-      <c r="G144" s="3"/>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V144" s="3"/>
+    </row>
+    <row r="145" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="8"/>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
       <c r="E145" s="8"/>
       <c r="F145" s="8"/>
-      <c r="G145" s="3"/>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V145" s="3"/>
+    </row>
+    <row r="146" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
       <c r="E146" s="8"/>
       <c r="F146" s="8"/>
-      <c r="G146" s="3"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V146" s="3"/>
+    </row>
+    <row r="147" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="8"/>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
       <c r="E147" s="8"/>
       <c r="F147" s="8"/>
-      <c r="G147" s="3"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V147" s="3"/>
+    </row>
+    <row r="148" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
       <c r="E148" s="8"/>
       <c r="F148" s="8"/>
-      <c r="G148" s="3"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V148" s="3"/>
+    </row>
+    <row r="149" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
       <c r="E149" s="8"/>
       <c r="F149" s="8"/>
-      <c r="G149" s="3"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V149" s="3"/>
+    </row>
+    <row r="150" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="8"/>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
       <c r="E150" s="8"/>
       <c r="F150" s="8"/>
-      <c r="G150" s="3"/>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V150" s="3"/>
+    </row>
+    <row r="151" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="8"/>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
       <c r="E151" s="8"/>
       <c r="F151" s="8"/>
-      <c r="G151" s="3"/>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V151" s="3"/>
+    </row>
+    <row r="152" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="8"/>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
       <c r="E152" s="8"/>
       <c r="F152" s="8"/>
-      <c r="G152" s="3"/>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V152" s="3"/>
+    </row>
+    <row r="153" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="8"/>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
       <c r="E153" s="8"/>
       <c r="F153" s="8"/>
-      <c r="G153" s="3"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V153" s="3"/>
+    </row>
+    <row r="154" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
       <c r="E154" s="8"/>
       <c r="F154" s="8"/>
-      <c r="G154" s="3"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V154" s="3"/>
+    </row>
+    <row r="155" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="8"/>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
       <c r="E155" s="8"/>
       <c r="F155" s="8"/>
-      <c r="G155" s="3"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V155" s="3"/>
+    </row>
+    <row r="156" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
       <c r="E156" s="8"/>
       <c r="F156" s="8"/>
-      <c r="G156" s="3"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V156" s="3"/>
+    </row>
+    <row r="157" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
       <c r="D157" s="8"/>
       <c r="E157" s="8"/>
       <c r="F157" s="8"/>
-      <c r="G157" s="3"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V157" s="3"/>
+    </row>
+    <row r="158" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="8"/>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
       <c r="D158" s="8"/>
       <c r="E158" s="8"/>
       <c r="F158" s="8"/>
-      <c r="G158" s="3"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V158" s="3"/>
+    </row>
+    <row r="159" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="8"/>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
       <c r="F159" s="8"/>
-      <c r="G159" s="3"/>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V159" s="3"/>
+    </row>
+    <row r="160" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="8"/>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
       <c r="D160" s="8"/>
       <c r="E160" s="8"/>
       <c r="F160" s="8"/>
-      <c r="G160" s="3"/>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V160" s="3"/>
+    </row>
+    <row r="161" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="8"/>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
       <c r="D161" s="8"/>
       <c r="E161" s="8"/>
       <c r="F161" s="8"/>
-      <c r="G161" s="3"/>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V161" s="3"/>
+    </row>
+    <row r="162" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
       <c r="D162" s="8"/>
       <c r="E162" s="8"/>
       <c r="F162" s="8"/>
-      <c r="G162" s="3"/>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V162" s="3"/>
+    </row>
+    <row r="163" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="8"/>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
       <c r="D163" s="8"/>
       <c r="E163" s="8"/>
       <c r="F163" s="8"/>
-      <c r="G163" s="3"/>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V163" s="3"/>
+    </row>
+    <row r="164" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="8"/>
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
       <c r="D164" s="8"/>
       <c r="E164" s="8"/>
       <c r="F164" s="8"/>
-      <c r="G164" s="3"/>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V164" s="3"/>
+    </row>
+    <row r="165" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="8"/>
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
       <c r="D165" s="8"/>
       <c r="E165" s="8"/>
       <c r="F165" s="8"/>
-      <c r="G165" s="3"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V165" s="3"/>
+    </row>
+    <row r="166" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="8"/>
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
       <c r="D166" s="8"/>
       <c r="E166" s="8"/>
       <c r="F166" s="8"/>
-      <c r="G166" s="3"/>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V166" s="3"/>
+    </row>
+    <row r="167" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="8"/>
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
       <c r="D167" s="8"/>
       <c r="E167" s="8"/>
       <c r="F167" s="8"/>
-      <c r="G167" s="3"/>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V167" s="3"/>
+    </row>
+    <row r="168" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="8"/>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
       <c r="D168" s="8"/>
       <c r="E168" s="8"/>
       <c r="F168" s="8"/>
-      <c r="G168" s="3"/>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V168" s="3"/>
+    </row>
+    <row r="169" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="8"/>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
       <c r="D169" s="8"/>
       <c r="E169" s="8"/>
       <c r="F169" s="8"/>
-      <c r="G169" s="3"/>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V169" s="3"/>
+    </row>
+    <row r="170" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="8"/>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
       <c r="D170" s="8"/>
       <c r="E170" s="8"/>
       <c r="F170" s="8"/>
-      <c r="G170" s="3"/>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V170" s="3"/>
+    </row>
+    <row r="171" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="8"/>
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
       <c r="D171" s="8"/>
       <c r="E171" s="8"/>
       <c r="F171" s="8"/>
-      <c r="G171" s="3"/>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V171" s="3"/>
+    </row>
+    <row r="172" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="8"/>
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
       <c r="D172" s="8"/>
       <c r="E172" s="8"/>
       <c r="F172" s="8"/>
-      <c r="G172" s="3"/>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V172" s="3"/>
+    </row>
+    <row r="173" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="8"/>
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
       <c r="D173" s="8"/>
       <c r="E173" s="8"/>
       <c r="F173" s="8"/>
-      <c r="G173" s="3"/>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V173" s="3"/>
+    </row>
+    <row r="174" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="8"/>
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
       <c r="D174" s="8"/>
       <c r="E174" s="8"/>
       <c r="F174" s="8"/>
-      <c r="G174" s="3"/>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V174" s="3"/>
+    </row>
+    <row r="175" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="8"/>
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
       <c r="D175" s="8"/>
       <c r="E175" s="8"/>
       <c r="F175" s="8"/>
-      <c r="G175" s="3"/>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V175" s="3"/>
+    </row>
+    <row r="176" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="8"/>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
       <c r="D176" s="8"/>
       <c r="E176" s="8"/>
       <c r="F176" s="8"/>
-      <c r="G176" s="3"/>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V176" s="3"/>
+    </row>
+    <row r="177" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="8"/>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
       <c r="D177" s="8"/>
       <c r="E177" s="8"/>
       <c r="F177" s="8"/>
-      <c r="G177" s="3"/>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V177" s="3"/>
+    </row>
+    <row r="178" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
       <c r="D178" s="8"/>
       <c r="E178" s="8"/>
       <c r="F178" s="8"/>
-      <c r="G178" s="3"/>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V178" s="3"/>
+    </row>
+    <row r="179" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="8"/>
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
       <c r="D179" s="8"/>
       <c r="E179" s="8"/>
       <c r="F179" s="8"/>
-      <c r="G179" s="3"/>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V179" s="3"/>
+    </row>
+    <row r="180" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="8"/>
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
       <c r="D180" s="8"/>
       <c r="E180" s="8"/>
       <c r="F180" s="8"/>
-      <c r="G180" s="3"/>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V180" s="3"/>
+    </row>
+    <row r="181" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="8"/>
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
       <c r="D181" s="8"/>
       <c r="E181" s="8"/>
       <c r="F181" s="8"/>
-      <c r="G181" s="3"/>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V181" s="3"/>
+    </row>
+    <row r="182" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
       <c r="D182" s="8"/>
       <c r="E182" s="8"/>
       <c r="F182" s="8"/>
-      <c r="G182" s="3"/>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V182" s="3"/>
+    </row>
+    <row r="183" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
       <c r="D183" s="8"/>
       <c r="E183" s="8"/>
       <c r="F183" s="8"/>
-      <c r="G183" s="3"/>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V183" s="3"/>
+    </row>
+    <row r="184" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
       <c r="F184" s="8"/>
-      <c r="G184" s="3"/>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V184" s="3"/>
+    </row>
+    <row r="185" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="8"/>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
       <c r="D185" s="8"/>
       <c r="E185" s="8"/>
       <c r="F185" s="8"/>
-      <c r="G185" s="3"/>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V185" s="3"/>
+    </row>
+    <row r="186" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
       <c r="D186" s="8"/>
       <c r="E186" s="8"/>
       <c r="F186" s="8"/>
-      <c r="G186" s="3"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V186" s="3"/>
+    </row>
+    <row r="187" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
       <c r="D187" s="8"/>
       <c r="E187" s="8"/>
       <c r="F187" s="8"/>
-      <c r="G187" s="3"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V187" s="3"/>
+    </row>
+    <row r="188" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
       <c r="D188" s="8"/>
       <c r="E188" s="8"/>
       <c r="F188" s="8"/>
-      <c r="G188" s="3"/>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V188" s="3"/>
+    </row>
+    <row r="189" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
       <c r="D189" s="8"/>
       <c r="E189" s="8"/>
       <c r="F189" s="8"/>
-      <c r="G189" s="3"/>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V189" s="3"/>
+    </row>
+    <row r="190" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="8"/>
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
       <c r="D190" s="8"/>
       <c r="E190" s="8"/>
       <c r="F190" s="8"/>
-      <c r="G190" s="3"/>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V190" s="3"/>
+    </row>
+    <row r="191" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="8"/>
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
       <c r="D191" s="8"/>
       <c r="E191" s="8"/>
       <c r="F191" s="8"/>
-      <c r="G191" s="3"/>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V191" s="3"/>
+    </row>
+    <row r="192" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="8"/>
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
       <c r="D192" s="8"/>
       <c r="E192" s="8"/>
       <c r="F192" s="8"/>
-      <c r="G192" s="3"/>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V192" s="3"/>
+    </row>
+    <row r="193" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
       <c r="D193" s="8"/>
       <c r="E193" s="8"/>
       <c r="F193" s="8"/>
-      <c r="G193" s="3"/>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V193" s="3"/>
+    </row>
+    <row r="194" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
       <c r="D194" s="8"/>
       <c r="E194" s="8"/>
       <c r="F194" s="8"/>
-      <c r="G194" s="3"/>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V194" s="3"/>
+    </row>
+    <row r="195" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="8"/>
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
       <c r="D195" s="8"/>
       <c r="E195" s="8"/>
       <c r="F195" s="8"/>
-      <c r="G195" s="3"/>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V195" s="3"/>
+    </row>
+    <row r="196" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
       <c r="D196" s="8"/>
       <c r="E196" s="8"/>
       <c r="F196" s="8"/>
-      <c r="G196" s="3"/>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V196" s="3"/>
+    </row>
+    <row r="197" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="8"/>
       <c r="B197" s="8"/>
       <c r="C197" s="8"/>
       <c r="D197" s="8"/>
       <c r="E197" s="8"/>
       <c r="F197" s="8"/>
-      <c r="G197" s="3"/>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V197" s="3"/>
+    </row>
+    <row r="198" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="8"/>
       <c r="B198" s="8"/>
       <c r="C198" s="8"/>
       <c r="D198" s="8"/>
       <c r="E198" s="8"/>
       <c r="F198" s="8"/>
-      <c r="G198" s="3"/>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V198" s="3"/>
+    </row>
+    <row r="199" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
       <c r="D199" s="8"/>
       <c r="E199" s="8"/>
       <c r="F199" s="8"/>
-      <c r="G199" s="3"/>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V199" s="3"/>
+    </row>
+    <row r="200" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="8"/>
       <c r="B200" s="8"/>
       <c r="C200" s="8"/>
       <c r="D200" s="8"/>
       <c r="E200" s="8"/>
       <c r="F200" s="8"/>
-      <c r="G200" s="3"/>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="V200" s="3"/>
+    </row>
+    <row r="201" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="10"/>
       <c r="B201" s="10"/>
       <c r="C201" s="10"/>
       <c r="D201" s="10"/>
       <c r="E201" s="10"/>
       <c r="F201" s="11"/>
-      <c r="G201" s="3"/>
+      <c r="V201" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
-  <dataValidations count="2">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="無効なステータス" error="サポートされているステータスを選択してください。" sqref="E2:E1048576" xr:uid="{AE54C896-4182-499E-B11F-3D57E93582E8}">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="無効なID" error="IDは0より大きい整数である必要があります。" sqref="A2:A1048576" xr:uid="{CCA7D833-6739-4C5E-A174-5BF3207240BB}">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576" xr:uid="{E0E464C0-59A9-4118-91AA-F8F3503E2FA5}">
+      <formula1>"Verbose, Trace, Information, Warning, Error, Critical, Off"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:S1048576" xr:uid="{709F1C42-7DA4-413C-AD6B-9A3D5700BE5F}">
+      <formula1>0</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{2E0A79E6-22BF-46B1-98A1-00527F585E56}">
+      <formula1>"NonProduction, Attended, Unattended, Studio, Development, StudioX, Headless, StudioPro, TestAutomation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:J1048576 M2:M1048576 T2:U1048576 O2:P1048576" xr:uid="{3BA63961-21AA-4A71-AD30-18A582299C12}">
+      <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>